<commit_message>
Rework week 6, add graphs for true wins
</commit_message>
<xml_diff>
--- a/power_rankings_history/2023/week_6/Week-6-Power-Rankings-Final.xlsx
+++ b/power_rankings_history/2023/week_6/Week-6-Power-Rankings-Final.xlsx
@@ -2,25 +2,59 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
-  <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rthotaku/playground/sleeper-league-power-rankings/power_rankings_history/2023/week_6/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{1253D0F9-710B-084D-AA26-C6B8971B9B95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{0A954DDE-B430-A240-A647-7DCCCB07F69D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3900" yWindow="2200" windowWidth="28040" windowHeight="17440"/>
   </bookViews>
   <sheets>
     <sheet name="Week-6-Power-Rankings" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">'Week-6-Power-Rankings'!$E$2:$E$10</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">'Week-6-Power-Rankings'!$E$2:$E$9</definedName>
+    <definedName name="_xlchart.v1.13" hidden="1">'Week-6-Power-Rankings'!$A$2:$O$2</definedName>
+    <definedName name="_xlchart.v1.14" hidden="1">'Week-6-Power-Rankings'!$A$3:$O$3</definedName>
+    <definedName name="_xlchart.v1.15" hidden="1">'Week-6-Power-Rankings'!$A$4:$O$4</definedName>
+    <definedName name="_xlchart.v1.16" hidden="1">'Week-6-Power-Rankings'!$A$5:$O$5</definedName>
+    <definedName name="_xlchart.v1.17" hidden="1">'Week-6-Power-Rankings'!$A$6:$O$6</definedName>
+    <definedName name="_xlchart.v1.18" hidden="1">'Week-6-Power-Rankings'!$A$7:$O$7</definedName>
+    <definedName name="_xlchart.v1.19" hidden="1">'Week-6-Power-Rankings'!$A$8:$O$8</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">'Week-6-Power-Rankings'!$G$2:$G$9</definedName>
+    <definedName name="_xlchart.v1.20" hidden="1">'Week-6-Power-Rankings'!$A$9:$O$9</definedName>
+    <definedName name="_xlchart.v1.21" hidden="1">'Week-6-Power-Rankings'!$E$2:$E$10</definedName>
+    <definedName name="_xlchart.v1.22" hidden="1">'Week-6-Power-Rankings'!$E$2:$E$9</definedName>
+    <definedName name="_xlchart.v1.23" hidden="1">'Week-6-Power-Rankings'!$G$2:$G$9</definedName>
+    <definedName name="_xlchart.v1.24" hidden="1">'Week-6-Power-Rankings'!$N$2:$N$9</definedName>
+    <definedName name="_xlchart.v1.25" hidden="1">'Week-6-Power-Rankings'!$O$2:$O$9</definedName>
+    <definedName name="_xlchart.v1.26" hidden="1">'Week-6-Power-Rankings'!$B$2:$B$9</definedName>
+    <definedName name="_xlchart.v1.27" hidden="1">'Week-6-Power-Rankings'!$E$2:$E$10</definedName>
+    <definedName name="_xlchart.v1.28" hidden="1">'Week-6-Power-Rankings'!$E$2:$E$9</definedName>
+    <definedName name="_xlchart.v1.29" hidden="1">'Week-6-Power-Rankings'!$G$2:$G$9</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">'Week-6-Power-Rankings'!$N$2:$N$9</definedName>
+    <definedName name="_xlchart.v1.30" hidden="1">'Week-6-Power-Rankings'!$I$2:$I$9</definedName>
+    <definedName name="_xlchart.v1.31" hidden="1">'Week-6-Power-Rankings'!$O$2:$O$9</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">'Week-6-Power-Rankings'!$O$2:$O$9</definedName>
+    <definedName name="_xlchart.v2.10" hidden="1">'Week-6-Power-Rankings'!$A$7:$O$7</definedName>
+    <definedName name="_xlchart.v2.11" hidden="1">'Week-6-Power-Rankings'!$A$8:$O$8</definedName>
+    <definedName name="_xlchart.v2.12" hidden="1">'Week-6-Power-Rankings'!$A$9:$O$9</definedName>
+    <definedName name="_xlchart.v2.5" hidden="1">'Week-6-Power-Rankings'!$A$2:$O$2</definedName>
+    <definedName name="_xlchart.v2.6" hidden="1">'Week-6-Power-Rankings'!$A$3:$O$3</definedName>
+    <definedName name="_xlchart.v2.7" hidden="1">'Week-6-Power-Rankings'!$A$4:$O$4</definedName>
+    <definedName name="_xlchart.v2.8" hidden="1">'Week-6-Power-Rankings'!$A$5:$O$5</definedName>
+    <definedName name="_xlchart.v2.9" hidden="1">'Week-6-Power-Rankings'!$A$6:$O$6</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>POWER RANK</t>
   </si>
@@ -55,6 +89,9 @@
     <t>Recent Wins Rank</t>
   </si>
   <si>
+    <t>True Wins</t>
+  </si>
+  <si>
     <t>Consistency Rating</t>
   </si>
   <si>
@@ -67,34 +104,19 @@
     <t>rahoolramesh</t>
   </si>
   <si>
-    <t>0.1021885768098603</t>
-  </si>
-  <si>
     <t>TATEZ</t>
   </si>
   <si>
-    <t>0.10411702440690415</t>
-  </si>
-  <si>
     <t>arpanchavan00</t>
   </si>
   <si>
-    <t>0.1613987864729734</t>
-  </si>
-  <si>
     <t>rohandang856</t>
   </si>
   <si>
-    <t>0.1291009443867172</t>
-  </si>
-  <si>
     <t>rowthehill</t>
   </si>
   <si>
     <t>umangchavan</t>
-  </si>
-  <si>
-    <t>0.12081471471278593</t>
   </si>
   <si>
     <t>joooon</t>
@@ -584,9 +606,8 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
@@ -633,7 +654,14 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -647,16 +675,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:N9" totalsRowShown="0">
-  <autoFilter ref="A1:N9"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:O9" totalsRowShown="0">
+  <autoFilter ref="A1:O9"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:O9">
     <sortCondition ref="A1:A9"/>
   </sortState>
-  <tableColumns count="14">
+  <tableColumns count="15">
     <tableColumn id="1" name="POWER RANK"/>
     <tableColumn id="2" name="Member"/>
     <tableColumn id="3" name="POWER RANK VALUE"/>
-    <tableColumn id="4" name="PPG"/>
+    <tableColumn id="4" name="PPG" dataDxfId="1"/>
     <tableColumn id="5" name="PPG Rank"/>
     <tableColumn id="6" name="Wins"/>
     <tableColumn id="7" name="Win Rank"/>
@@ -664,9 +692,10 @@
     <tableColumn id="9" name="Overall Win Rank"/>
     <tableColumn id="10" name="Recent Wins"/>
     <tableColumn id="11" name="Recent Wins Rank"/>
-    <tableColumn id="12" name="Consistency Rating"/>
-    <tableColumn id="13" name="Consistency Rank"/>
-    <tableColumn id="14" name="ROS Roster Rank"/>
+    <tableColumn id="12" name="True Wins" dataDxfId="0"/>
+    <tableColumn id="13" name="Consistency Rating"/>
+    <tableColumn id="14" name="Consistency Rank"/>
+    <tableColumn id="15" name="ROS Roster Rank"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -969,30 +998,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N9"/>
+  <dimension ref="A1:O9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.1640625" customWidth="1"/>
     <col min="2" max="2" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.1640625" customWidth="1"/>
+    <col min="5" max="5" width="11.5" customWidth="1"/>
     <col min="7" max="7" width="11.5" customWidth="1"/>
     <col min="8" max="8" width="14.1640625" customWidth="1"/>
     <col min="9" max="9" width="18" customWidth="1"/>
     <col min="10" max="10" width="13.83203125" customWidth="1"/>
     <col min="11" max="11" width="18.5" customWidth="1"/>
-    <col min="12" max="12" width="19" customWidth="1"/>
-    <col min="13" max="13" width="17.83203125" customWidth="1"/>
-    <col min="14" max="14" width="17.5" customWidth="1"/>
+    <col min="12" max="12" width="11.83203125" customWidth="1"/>
+    <col min="13" max="13" width="19" customWidth="1"/>
+    <col min="14" max="14" width="17.83203125" customWidth="1"/>
+    <col min="15" max="15" width="17.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1035,8 +1064,11 @@
       <c r="N1" t="s">
         <v>13</v>
       </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1070,27 +1102,30 @@
       <c r="K2">
         <v>2</v>
       </c>
-      <c r="L2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="M2">
+      <c r="L2" s="1">
+        <v>5.2857142857142803</v>
+      </c>
+      <c r="M2" s="1">
+        <v>0.104117024406904</v>
+      </c>
+      <c r="N2">
         <v>5</v>
       </c>
-      <c r="N2">
+      <c r="O2">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C3">
         <v>1.24</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="1">
         <v>389.43333089192703</v>
       </c>
       <c r="E3">
@@ -1114,22 +1149,25 @@
       <c r="K3">
         <v>1</v>
       </c>
-      <c r="L3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="M3">
+      <c r="L3" s="1">
+        <v>3.71428571428571</v>
+      </c>
+      <c r="M3" s="1">
+        <v>0.12910094438671699</v>
+      </c>
+      <c r="N3">
         <v>7</v>
       </c>
-      <c r="N3">
+      <c r="O3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C4">
         <v>1.67</v>
@@ -1158,27 +1196,30 @@
       <c r="K4">
         <v>2</v>
       </c>
-      <c r="L4">
+      <c r="L4" s="1">
+        <v>3.4285714285714199</v>
+      </c>
+      <c r="M4">
         <v>6.3919352818090899E-2</v>
       </c>
-      <c r="M4">
+      <c r="N4">
         <v>1</v>
       </c>
-      <c r="N4">
+      <c r="O4">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C5">
         <v>1.79</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="1">
         <v>374.743333333333</v>
       </c>
       <c r="E5">
@@ -1202,22 +1243,25 @@
       <c r="K5">
         <v>2</v>
       </c>
-      <c r="L5">
+      <c r="L5" s="1">
+        <v>3.4285714285714199</v>
+      </c>
+      <c r="M5">
         <v>7.29972473523645E-2</v>
       </c>
-      <c r="M5">
+      <c r="N5">
         <v>3</v>
       </c>
-      <c r="N5">
+      <c r="O5">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C6">
         <v>3.89</v>
@@ -1246,27 +1290,30 @@
       <c r="K6">
         <v>8</v>
       </c>
-      <c r="L6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="M6">
+      <c r="L6" s="1">
+        <v>3.1428571428571401</v>
+      </c>
+      <c r="M6" s="1">
+        <v>0.10218857680986</v>
+      </c>
+      <c r="N6">
         <v>4</v>
       </c>
-      <c r="N6">
+      <c r="O6">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C7">
         <v>3.89</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="1">
         <v>356.28666666666601</v>
       </c>
       <c r="E7">
@@ -1290,27 +1337,30 @@
       <c r="K7">
         <v>2</v>
       </c>
-      <c r="L7" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="M7">
+      <c r="L7" s="1">
+        <v>2.2857142857142798</v>
+      </c>
+      <c r="M7" s="1">
+        <v>0.120814714712785</v>
+      </c>
+      <c r="N7">
         <v>6</v>
       </c>
-      <c r="N7">
+      <c r="O7">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C8">
         <v>4.0199999999999996</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="1">
         <v>361.38666666666597</v>
       </c>
       <c r="E8">
@@ -1334,27 +1384,30 @@
       <c r="K8">
         <v>2</v>
       </c>
-      <c r="L8" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="M8">
+      <c r="L8" s="1">
+        <v>2.4285714285714199</v>
+      </c>
+      <c r="M8" s="1">
+        <v>0.16139878647297301</v>
+      </c>
+      <c r="N8">
         <v>8</v>
       </c>
-      <c r="N8">
+      <c r="O8">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C9">
         <v>4.96</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="1">
         <v>313.20666666666602</v>
       </c>
       <c r="E9">
@@ -1378,13 +1431,16 @@
       <c r="K9">
         <v>7</v>
       </c>
-      <c r="L9">
+      <c r="L9" s="1">
+        <v>0.28571428571428498</v>
+      </c>
+      <c r="M9">
         <v>6.9541401999901206E-2</v>
       </c>
-      <c r="M9">
+      <c r="N9">
         <v>2</v>
       </c>
-      <c r="N9">
+      <c r="O9">
         <v>8</v>
       </c>
     </row>

</xml_diff>